<commit_message>
Updated SQM sheet. Test report link needs to be updated
</commit_message>
<xml_diff>
--- a/docs/design/GC2115/SW-SQM-GC2115-R1.xlsx
+++ b/docs/design/GC2115/SW-SQM-GC2115-R1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098C8FD9-C9E7-4CAF-AFB5-48AC700C671A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4F9330-4713-47ED-A10A-8B5AB2B73CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,7 +344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="134">
   <si>
     <t>SEDEMAC</t>
   </si>
@@ -705,12 +705,6 @@
 Ramachandran S</t>
   </si>
   <si>
-    <t>11 warnings</t>
-  </si>
-  <si>
-    <t>36c97b6</t>
-  </si>
-  <si>
     <t>SW_GC2X_NEW</t>
   </si>
   <si>
@@ -726,22 +720,10 @@
     <t>improvement/STB_fault_detection</t>
   </si>
   <si>
-    <t>963ba8a</t>
-  </si>
-  <si>
     <t>Aditya Joshi</t>
   </si>
   <si>
-    <t>01 / 24-06-2024</t>
-  </si>
-  <si>
     <t>SW-SQM-GC2115-R1</t>
-  </si>
-  <si>
-    <t>Software Quality Metric For : GC2115 R1 (Firmware : R0.27)</t>
-  </si>
-  <si>
-    <t>Test reports of R0v03, R0v08 and R0v20 are available in OHA+OHSW Teams chat</t>
   </si>
   <si>
     <t>Test cases updated by :
@@ -759,13 +741,28 @@
     <t>Release note</t>
   </si>
   <si>
-    <t>Release commit for R0V27 is in the master branch in the new repo</t>
-  </si>
-  <si>
     <t>master</t>
   </si>
   <si>
-    <t>Issues in this Jira project upto (and including) GC2115-111</t>
+    <t>7aa56c4</t>
+  </si>
+  <si>
+    <t>Release commit for R0V29 is in the master branch in the new repo</t>
+  </si>
+  <si>
+    <t>Issues in this Jira project upto (and including) GC2115-116</t>
+  </si>
+  <si>
+    <t>Test reports of R0v03, R0v08, R0v20 and R0V27 are available in OHA+OHSW Teams chat</t>
+  </si>
+  <si>
+    <t>Software Quality Metric For : GC2115 R1 (Firmware : R0.29)</t>
+  </si>
+  <si>
+    <t>01 / 27-06-2024</t>
+  </si>
+  <si>
+    <t>ef947a7</t>
   </si>
 </sst>
 </file>
@@ -1116,14 +1113,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1558,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50:H50"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,7 +1586,7 @@
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="51" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D1" s="52"/>
       <c r="E1" s="43" t="s">
@@ -1597,7 +1594,7 @@
       </c>
       <c r="F1" s="44"/>
       <c r="G1" s="60" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H1" s="60"/>
       <c r="N1" t="s">
@@ -1614,7 +1611,7 @@
       </c>
       <c r="F2" s="44"/>
       <c r="G2" s="63" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="H2" s="63"/>
       <c r="L2" t="s">
@@ -1668,7 +1665,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="61" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D4" s="61"/>
       <c r="E4" s="61"/>
@@ -1735,7 +1732,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="61" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D6" s="61"/>
       <c r="E6" s="61"/>
@@ -1775,7 +1772,7 @@
       </c>
       <c r="B8" s="60"/>
       <c r="C8" s="62" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D8" s="62"/>
       <c r="E8" s="62"/>
@@ -1792,14 +1789,14 @@
         <v>37</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="10" t="s">
         <v>37</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="10"/>
@@ -1811,14 +1808,14 @@
         <v>38</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E10" s="73"/>
       <c r="F10" s="10" t="s">
         <v>38</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="10"/>
@@ -1830,14 +1827,14 @@
         <v>39</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="10" t="s">
         <v>39</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="10"/>
@@ -1849,14 +1846,14 @@
         <v>40</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="10" t="s">
         <v>40</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="10"/>
@@ -1912,7 +1909,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H15" s="25"/>
       <c r="R15" s="13" t="s">
@@ -1935,8 +1932,8 @@
         <f>IF(D16&gt;=60,(F15*2*D16/100),0)</f>
         <v>7.2</v>
       </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="34"/>
       <c r="R16" s="12" t="s">
         <v>50</v>
       </c>
@@ -2038,7 +2035,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H21" s="20"/>
       <c r="R21" s="12" t="s">
@@ -2061,8 +2058,8 @@
         <f>IF(D22="Yes",2,0)</f>
         <v>0</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="34"/>
       <c r="R22" s="12" t="s">
         <v>56</v>
       </c>
@@ -2201,8 +2198,8 @@
         <f>IF(D28="Yes",1,IF(D28="Not Applicable",0.5,0))</f>
         <v>0</v>
       </c>
-      <c r="G28" s="33"/>
-      <c r="H28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="34"/>
       <c r="R28" s="12" t="s">
         <v>62</v>
       </c>
@@ -2291,10 +2288,10 @@
         <f>IF(D32="Yes",1,IF(D32="Not Applicable",0.5,0))</f>
         <v>1</v>
       </c>
-      <c r="G32" s="34" t="s">
+      <c r="G32" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="H32" s="35"/>
+      <c r="H32" s="34"/>
       <c r="R32" s="12" t="s">
         <v>62</v>
       </c>
@@ -2339,8 +2336,8 @@
         <f>IF(D34=P2,5,(IF(D34=P3,4,(IF(D34=P4,3,(IF(D34=P5,2,0)))))))</f>
         <v>4</v>
       </c>
-      <c r="G34" s="33"/>
-      <c r="H34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="34"/>
       <c r="R34" s="12" t="s">
         <v>68</v>
       </c>
@@ -2385,8 +2382,8 @@
         <f>IF(D36=N2,0,IF(D36=N1,1,2))</f>
         <v>0</v>
       </c>
-      <c r="G36" s="33"/>
-      <c r="H36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="34"/>
       <c r="R36" s="12" t="s">
         <v>72</v>
       </c>
@@ -2400,16 +2397,14 @@
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="9" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3">
         <f>IF(D37="Yes",3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>115</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G37" s="20"/>
       <c r="H37" s="21"/>
       <c r="R37" s="12" t="s">
         <v>74</v>
@@ -2432,7 +2427,7 @@
         <v>5</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H38" s="21"/>
       <c r="R38" s="12" t="s">
@@ -2456,7 +2451,7 @@
         <v>5</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H39" s="21"/>
       <c r="R39" s="12" t="s">
@@ -2504,7 +2499,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H41" s="21"/>
       <c r="R41" s="12" t="s">
@@ -2770,7 +2765,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="25" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H53" s="25"/>
       <c r="R53" s="12" t="s">
@@ -2802,7 +2797,7 @@
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F55" s="3">
         <f>F16+SUM(F19:F54)-F42-F43</f>
-        <v>82.2</v>
+        <v>85.2</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
@@ -2811,7 +2806,7 @@
       </c>
       <c r="D58" s="4">
         <f>F55</f>
-        <v>82.2</v>
+        <v>85.2</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
@@ -2995,7 +2990,7 @@
     <hyperlink ref="G9:H9" r:id="rId2" display="SW_GC2X" xr:uid="{EC7AD197-7C66-480C-8362-1B0BD2425E07}"/>
     <hyperlink ref="G10:H10" r:id="rId3" display=" gc2k-bsp" xr:uid="{69D5A13C-99D6-4281-B6C6-70406113334C}"/>
     <hyperlink ref="G11:H11" r:id="rId4" display="improvement/STB_fault_detection" xr:uid="{4A617C9E-732C-4FE8-A242-62AC223E5AE6}"/>
-    <hyperlink ref="G12:H12" r:id="rId5" display="963ba8a" xr:uid="{347D5B0A-60B0-4906-B6FD-3DE0171ECDC9}"/>
+    <hyperlink ref="G12:H12" r:id="rId5" display="ef947a7" xr:uid="{347D5B0A-60B0-4906-B6FD-3DE0171ECDC9}"/>
     <hyperlink ref="D10:E10" r:id="rId6" display="mnm_gc2115" xr:uid="{B77BA393-242E-46C1-BE40-46CBFDAB71A6}"/>
     <hyperlink ref="D11:E11" r:id="rId7" display="master" xr:uid="{9138540E-0134-4E6D-804F-9831A5D65242}"/>
     <hyperlink ref="G24:H24" r:id="rId8" display="Memory Map" xr:uid="{B7D64790-8F23-4097-B8E0-A3B0265F48FB}"/>
@@ -3003,7 +2998,7 @@
     <hyperlink ref="G26:H26" r:id="rId10" display="J1939 MAP" xr:uid="{39593EF7-6E84-4D3B-B4EA-C5A1B04AAB1A}"/>
     <hyperlink ref="G40:H40" r:id="rId11" display="Test Reports" xr:uid="{50A0996D-4FB1-44C9-865D-D4A56A82BC60}"/>
     <hyperlink ref="G30:H30" r:id="rId12" display="Confluence Page" xr:uid="{B8008C69-E29A-4C1E-8336-E18B1EB0AE96}"/>
-    <hyperlink ref="D12:E12" r:id="rId13" display="36c97b6" xr:uid="{E5380EF8-D403-43A4-822E-25F399F8076C}"/>
+    <hyperlink ref="D12:E12" r:id="rId13" display="7aa56c4" xr:uid="{E5380EF8-D403-43A4-822E-25F399F8076C}"/>
     <hyperlink ref="G53:H53" r:id="rId14" display="Release note" xr:uid="{BE36B37C-0323-4886-AF54-41385AE8401D}"/>
     <hyperlink ref="G15:H15" r:id="rId15" display="Issues in this Jira project upto (and including) GC2115-111" xr:uid="{78770E48-7C9B-4D7C-BFD6-79F0F98CD449}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Updated SQM sheet and release note
</commit_message>
<xml_diff>
--- a/docs/design/GC2115/SW-SQM-GC2115-R1.xlsx
+++ b/docs/design/GC2115/SW-SQM-GC2115-R1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4F9330-4713-47ED-A10A-8B5AB2B73CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4391C585-FCDE-4C30-9860-2D9BA11ACD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1061,180 +1061,180 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1555,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,39 +1581,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="51" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="43" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="60" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="60"/>
+      <c r="H1" s="32"/>
       <c r="N1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="43" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="63" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="63"/>
+      <c r="H2" s="35"/>
       <c r="L2" t="s">
         <v>4</v>
       </c>
@@ -1631,18 +1631,18 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="43" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="63" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="63"/>
+      <c r="H3" s="35"/>
       <c r="L3" t="s">
         <v>11</v>
       </c>
@@ -1660,18 +1660,18 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="61" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
       <c r="J4" t="s">
         <v>17</v>
       </c>
@@ -1695,18 +1695,18 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="61" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
       <c r="J5" t="s">
         <v>24</v>
       </c>
@@ -1727,18 +1727,18 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="61" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
       <c r="J6" t="s">
         <v>25</v>
       </c>
@@ -1753,129 +1753,129 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="61" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="62" t="s">
+      <c r="B8" s="32"/>
+      <c r="C8" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="65"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="H9" s="16"/>
+      <c r="H9" s="45"/>
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="E10" s="73"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="H10" s="16"/>
+      <c r="H10" s="45"/>
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
-      <c r="B11" s="67"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="H11" s="16"/>
+      <c r="H11" s="45"/>
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="68"/>
-      <c r="B12" s="69"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="H12" s="16"/>
+      <c r="H12" s="45"/>
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="57"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="59"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="42"/>
+      <c r="C14" s="56"/>
       <c r="D14" s="1" t="s">
         <v>43</v>
       </c>
@@ -1883,10 +1883,10 @@
       <c r="F14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="42"/>
+      <c r="H14" s="56"/>
       <c r="R14" s="1" t="s">
         <v>46</v>
       </c>
@@ -1896,10 +1896,10 @@
       <c r="A15" s="2">
         <v>1</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="9" t="s">
         <v>14</v>
       </c>
@@ -1908,10 +1908,10 @@
         <f>IF(D15=O2,5,(IF(D15=O3,4,(IF(D15=O4,3,(IF(D15=O5,2,0)))))))</f>
         <v>4</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="H15" s="25"/>
+      <c r="H15" s="57"/>
       <c r="R15" s="13" t="s">
         <v>48</v>
       </c>
@@ -1920,10 +1920,10 @@
       <c r="A16" s="2">
         <v>2</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="54"/>
       <c r="D16" s="9">
         <v>90</v>
       </c>
@@ -1932,8 +1932,8 @@
         <f>IF(D16&gt;=60,(F15*2*D16/100),0)</f>
         <v>7.2</v>
       </c>
-      <c r="G16" s="35"/>
-      <c r="H16" s="34"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="52"/>
       <c r="R16" s="12" t="s">
         <v>50</v>
       </c>
@@ -1942,44 +1942,44 @@
       <c r="A17" s="2">
         <v>3</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="40"/>
+      <c r="C17" s="54"/>
       <c r="D17" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="21"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="58"/>
       <c r="R17" s="12"/>
     </row>
     <row r="18" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>4</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="40"/>
+      <c r="C18" s="54"/>
       <c r="D18" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="21"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="58"/>
       <c r="R18" s="12"/>
     </row>
     <row r="19" spans="1:18" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>5</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="40"/>
+      <c r="C19" s="54"/>
       <c r="D19" s="9" t="s">
         <v>6</v>
       </c>
@@ -1988,8 +1988,8 @@
         <f>IF(AND(OR(D17="Yes",AND(D18="Yes",D19="Yes")),NOT(D15="Not documented")),10,0)</f>
         <v>10</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="21"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="58"/>
       <c r="R19" s="12" t="s">
         <v>54</v>
       </c>
@@ -1998,10 +1998,10 @@
       <c r="A20" s="2">
         <v>6</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="32"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="9" t="s">
         <v>13</v>
       </c>
@@ -2010,10 +2010,10 @@
         <f>IF(D20="Yes",2,0)</f>
         <v>2</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="H20" s="25"/>
+      <c r="H20" s="57"/>
       <c r="R20" s="12" t="s">
         <v>56</v>
       </c>
@@ -2022,10 +2022,10 @@
       <c r="A21" s="2">
         <v>7</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="36"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="9" t="s">
         <v>13</v>
       </c>
@@ -2034,10 +2034,10 @@
         <f>IF(AND(D20="Yes",D21="Yes"),2,0)</f>
         <v>2</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="H21" s="20"/>
+      <c r="H21" s="48"/>
       <c r="R21" s="12" t="s">
         <v>58</v>
       </c>
@@ -2046,10 +2046,10 @@
       <c r="A22" s="2">
         <v>8</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="32"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="9" t="s">
         <v>6</v>
       </c>
@@ -2058,8 +2058,8 @@
         <f>IF(D22="Yes",2,0)</f>
         <v>0</v>
       </c>
-      <c r="G22" s="35"/>
-      <c r="H22" s="34"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="52"/>
       <c r="R22" s="12" t="s">
         <v>56</v>
       </c>
@@ -2068,10 +2068,10 @@
       <c r="A23" s="2">
         <v>9</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="36"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="9" t="s">
         <v>6</v>
       </c>
@@ -2080,8 +2080,8 @@
         <f>IF(AND(D22="Yes",D23="Yes"),2,0)</f>
         <v>0</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
       <c r="R23" s="12" t="s">
         <v>58</v>
       </c>
@@ -2090,10 +2090,10 @@
       <c r="A24" s="2">
         <v>10</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="32"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="9" t="s">
         <v>13</v>
       </c>
@@ -2102,10 +2102,10 @@
         <f>IF(D24="Yes",2,0)</f>
         <v>2</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="H24" s="25"/>
+      <c r="H24" s="57"/>
       <c r="R24" s="12" t="s">
         <v>56</v>
       </c>
@@ -2114,10 +2114,10 @@
       <c r="A25" s="2">
         <v>11</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="36"/>
+      <c r="C25" s="61"/>
       <c r="D25" s="9" t="s">
         <v>13</v>
       </c>
@@ -2126,10 +2126,10 @@
         <f>IF(AND(D24="Yes",D25="Yes"),2,0)</f>
         <v>2</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="20"/>
+      <c r="H25" s="48"/>
       <c r="R25" s="12" t="s">
         <v>58</v>
       </c>
@@ -2138,10 +2138,10 @@
       <c r="A26" s="2">
         <v>12</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="32"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="9" t="s">
         <v>13</v>
       </c>
@@ -2150,10 +2150,10 @@
         <f>IF(D26="Yes",1,IF(D26="Not Applicable",0.5,0))</f>
         <v>1</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="H26" s="25"/>
+      <c r="H26" s="57"/>
       <c r="R26" s="12" t="s">
         <v>62</v>
       </c>
@@ -2162,10 +2162,10 @@
       <c r="A27" s="2">
         <v>13</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="36"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="9" t="s">
         <v>13</v>
       </c>
@@ -2174,10 +2174,10 @@
         <f>IF(AND(D26="Yes",D27="Yes"),1,0)</f>
         <v>1</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="H27" s="20"/>
+      <c r="H27" s="48"/>
       <c r="R27" s="12" t="s">
         <v>63</v>
       </c>
@@ -2186,10 +2186,10 @@
       <c r="A28" s="2">
         <v>14</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="32"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="9" t="s">
         <v>6</v>
       </c>
@@ -2198,8 +2198,8 @@
         <f>IF(D28="Yes",1,IF(D28="Not Applicable",0.5,0))</f>
         <v>0</v>
       </c>
-      <c r="G28" s="35"/>
-      <c r="H28" s="34"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="52"/>
       <c r="R28" s="12" t="s">
         <v>62</v>
       </c>
@@ -2208,10 +2208,10 @@
       <c r="A29" s="2">
         <v>15</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="36"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="9" t="s">
         <v>6</v>
       </c>
@@ -2220,8 +2220,8 @@
         <f>IF(AND(D28="Yes",D29="Yes"),1,0)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
       <c r="R29" s="12" t="s">
         <v>63</v>
       </c>
@@ -2230,10 +2230,10 @@
       <c r="A30" s="2">
         <v>16</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="32"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="9" t="s">
         <v>13</v>
       </c>
@@ -2242,10 +2242,10 @@
         <f>IF(D30="Yes",1,IF(D30="Not Applicable",0.5,0))</f>
         <v>1</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="H30" s="16"/>
+      <c r="H30" s="45"/>
       <c r="R30" s="12" t="s">
         <v>62</v>
       </c>
@@ -2254,10 +2254,10 @@
       <c r="A31" s="2">
         <v>17</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="36"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="9" t="s">
         <v>6</v>
       </c>
@@ -2266,8 +2266,8 @@
         <f>IF(AND(D30="Yes",D31="Yes"),1,0)</f>
         <v>0</v>
       </c>
-      <c r="G31" s="37"/>
-      <c r="H31" s="38"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="63"/>
       <c r="R31" s="12" t="s">
         <v>63</v>
       </c>
@@ -2276,10 +2276,10 @@
       <c r="A32" s="2">
         <v>18</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="32"/>
+      <c r="C32" s="50"/>
       <c r="D32" s="9" t="s">
         <v>13</v>
       </c>
@@ -2288,10 +2288,10 @@
         <f>IF(D32="Yes",1,IF(D32="Not Applicable",0.5,0))</f>
         <v>1</v>
       </c>
-      <c r="G32" s="33" t="s">
+      <c r="G32" s="67" t="s">
         <v>111</v>
       </c>
-      <c r="H32" s="34"/>
+      <c r="H32" s="52"/>
       <c r="R32" s="12" t="s">
         <v>62</v>
       </c>
@@ -2300,10 +2300,10 @@
       <c r="A33" s="2">
         <v>19</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="32"/>
+      <c r="C33" s="50"/>
       <c r="D33" s="9" t="s">
         <v>13</v>
       </c>
@@ -2312,10 +2312,10 @@
         <f>IF(AND(D32="Yes",D33="Yes"),1,0)</f>
         <v>1</v>
       </c>
-      <c r="G33" s="20" t="s">
+      <c r="G33" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="H33" s="21"/>
+      <c r="H33" s="58"/>
       <c r="R33" s="12" t="s">
         <v>63</v>
       </c>
@@ -2324,10 +2324,10 @@
       <c r="A34" s="2">
         <v>20</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="27"/>
+      <c r="C34" s="60"/>
       <c r="D34" s="9" t="s">
         <v>15</v>
       </c>
@@ -2336,8 +2336,8 @@
         <f>IF(D34=P2,5,(IF(D34=P3,4,(IF(D34=P4,3,(IF(D34=P5,2,0)))))))</f>
         <v>4</v>
       </c>
-      <c r="G34" s="35"/>
-      <c r="H34" s="34"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="52"/>
       <c r="R34" s="12" t="s">
         <v>68</v>
       </c>
@@ -2346,10 +2346,10 @@
       <c r="A35" s="2">
         <v>21</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="27"/>
+      <c r="C35" s="60"/>
       <c r="D35" s="9" t="s">
         <v>13</v>
       </c>
@@ -2358,10 +2358,10 @@
         <f>IF(D35="Yes",10,0)</f>
         <v>10</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="G35" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="H35" s="21"/>
+      <c r="H35" s="58"/>
       <c r="R35" s="12" t="s">
         <v>70</v>
       </c>
@@ -2370,10 +2370,10 @@
       <c r="A36" s="2">
         <v>22</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="27"/>
+      <c r="C36" s="60"/>
       <c r="D36" s="9" t="s">
         <v>6</v>
       </c>
@@ -2382,8 +2382,8 @@
         <f>IF(D36=N2,0,IF(D36=N1,1,2))</f>
         <v>0</v>
       </c>
-      <c r="G36" s="35"/>
-      <c r="H36" s="34"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="52"/>
       <c r="R36" s="12" t="s">
         <v>72</v>
       </c>
@@ -2392,10 +2392,10 @@
       <c r="A37" s="2">
         <v>23</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="27"/>
+      <c r="C37" s="60"/>
       <c r="D37" s="9" t="s">
         <v>13</v>
       </c>
@@ -2404,8 +2404,8 @@
         <f>IF(D37="Yes",3,0)</f>
         <v>3</v>
       </c>
-      <c r="G37" s="20"/>
-      <c r="H37" s="21"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="58"/>
       <c r="R37" s="12" t="s">
         <v>74</v>
       </c>
@@ -2414,10 +2414,10 @@
       <c r="A38" s="2">
         <v>24</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="23"/>
+      <c r="C38" s="71"/>
       <c r="D38" s="9" t="s">
         <v>13</v>
       </c>
@@ -2426,10 +2426,10 @@
         <f>IF(D38="Yes",5,0)</f>
         <v>5</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="G38" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="H38" s="21"/>
+      <c r="H38" s="58"/>
       <c r="R38" s="12" t="s">
         <v>76</v>
       </c>
@@ -2438,10 +2438,10 @@
       <c r="A39" s="2">
         <v>25</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="23"/>
+      <c r="C39" s="71"/>
       <c r="D39" s="9" t="s">
         <v>13</v>
       </c>
@@ -2450,10 +2450,10 @@
         <f>IF(D39="Yes",5,0)</f>
         <v>5</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="G39" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="H39" s="21"/>
+      <c r="H39" s="58"/>
       <c r="R39" s="12" t="s">
         <v>76</v>
       </c>
@@ -2462,10 +2462,10 @@
       <c r="A40" s="2">
         <v>26</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="23"/>
+      <c r="C40" s="71"/>
       <c r="D40" s="9" t="s">
         <v>13</v>
       </c>
@@ -2474,10 +2474,10 @@
         <f>IF(D40="Yes",10,0)</f>
         <v>10</v>
       </c>
-      <c r="G40" s="25" t="s">
+      <c r="G40" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="H40" s="25"/>
+      <c r="H40" s="57"/>
       <c r="R40" s="12" t="s">
         <v>79</v>
       </c>
@@ -2486,10 +2486,10 @@
       <c r="A41" s="2">
         <v>27</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="19"/>
+      <c r="C41" s="66"/>
       <c r="D41" s="9" t="s">
         <v>13</v>
       </c>
@@ -2498,10 +2498,10 @@
         <f>IF(D41="Yes",9,0)</f>
         <v>9</v>
       </c>
-      <c r="G41" s="20" t="s">
+      <c r="G41" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="H41" s="21"/>
+      <c r="H41" s="58"/>
       <c r="R41" s="12" t="s">
         <v>81</v>
       </c>
@@ -2510,10 +2510,10 @@
       <c r="A42" s="2">
         <v>28</v>
       </c>
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="19"/>
+      <c r="C42" s="66"/>
       <c r="D42" s="9" t="s">
         <v>13</v>
       </c>
@@ -2522,8 +2522,8 @@
         <f t="shared" ref="F42:F54" si="0">IF(D42="Yes",1,0)</f>
         <v>1</v>
       </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="21"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="58"/>
       <c r="R42" s="12" t="s">
         <v>83</v>
       </c>
@@ -2532,10 +2532,10 @@
       <c r="A43" s="2">
         <v>29</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="24"/>
+      <c r="C43" s="68"/>
       <c r="D43" s="9">
         <v>0</v>
       </c>
@@ -2544,8 +2544,8 @@
         <f>IF(D43&gt;1,0,1)</f>
         <v>1</v>
       </c>
-      <c r="G43" s="20"/>
-      <c r="H43" s="21"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="58"/>
       <c r="R43" s="12" t="s">
         <v>85</v>
       </c>
@@ -2554,10 +2554,10 @@
       <c r="A44" s="2">
         <v>30</v>
       </c>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="19"/>
+      <c r="C44" s="66"/>
       <c r="D44" s="9" t="s">
         <v>6</v>
       </c>
@@ -2566,8 +2566,8 @@
         <f>IF(D44="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="G44" s="20"/>
-      <c r="H44" s="21"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="58"/>
       <c r="R44" s="12" t="s">
         <v>83</v>
       </c>
@@ -2576,10 +2576,10 @@
       <c r="A45" s="2">
         <v>31</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="19"/>
+      <c r="C45" s="66"/>
       <c r="D45" s="9" t="s">
         <v>13</v>
       </c>
@@ -2588,8 +2588,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G45" s="28"/>
-      <c r="H45" s="29"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="73"/>
       <c r="R45" s="12" t="s">
         <v>83</v>
       </c>
@@ -2598,10 +2598,10 @@
       <c r="A46" s="2">
         <v>32</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="19"/>
+      <c r="C46" s="66"/>
       <c r="D46" s="9" t="s">
         <v>13</v>
       </c>
@@ -2610,8 +2610,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
+      <c r="G46" s="64"/>
+      <c r="H46" s="64"/>
       <c r="R46" s="12" t="s">
         <v>83</v>
       </c>
@@ -2620,10 +2620,10 @@
       <c r="A47" s="2">
         <v>33</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="19"/>
+      <c r="C47" s="66"/>
       <c r="D47" s="9" t="s">
         <v>13</v>
       </c>
@@ -2632,8 +2632,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G47" s="20"/>
-      <c r="H47" s="21"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="58"/>
       <c r="R47" s="12" t="s">
         <v>83</v>
       </c>
@@ -2642,10 +2642,10 @@
       <c r="A48" s="2">
         <v>34</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="C48" s="19"/>
+      <c r="C48" s="66"/>
       <c r="D48" s="9" t="s">
         <v>13</v>
       </c>
@@ -2654,8 +2654,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G48" s="20"/>
-      <c r="H48" s="21"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="58"/>
       <c r="R48" s="12" t="s">
         <v>83</v>
       </c>
@@ -2664,10 +2664,10 @@
       <c r="A49" s="2">
         <v>35</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="C49" s="19"/>
+      <c r="C49" s="66"/>
       <c r="D49" s="9" t="s">
         <v>13</v>
       </c>
@@ -2676,8 +2676,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G49" s="20"/>
-      <c r="H49" s="21"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="58"/>
       <c r="R49" s="12" t="s">
         <v>83</v>
       </c>
@@ -2686,10 +2686,10 @@
       <c r="A50" s="2">
         <v>36</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="C50" s="24"/>
+      <c r="C50" s="68"/>
       <c r="D50" s="9" t="s">
         <v>13</v>
       </c>
@@ -2698,8 +2698,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="48"/>
       <c r="R50" s="12" t="s">
         <v>83</v>
       </c>
@@ -2708,10 +2708,10 @@
       <c r="A51" s="2">
         <v>37</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="C51" s="24"/>
+      <c r="C51" s="68"/>
       <c r="D51" s="9" t="s">
         <v>13</v>
       </c>
@@ -2720,8 +2720,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
       <c r="R51" s="12" t="s">
         <v>83</v>
       </c>
@@ -2730,10 +2730,10 @@
       <c r="A52" s="2">
         <v>38</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="C52" s="24"/>
+      <c r="C52" s="68"/>
       <c r="D52" s="9" t="s">
         <v>13</v>
       </c>
@@ -2742,8 +2742,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="48"/>
       <c r="R52" s="12" t="s">
         <v>83</v>
       </c>
@@ -2752,10 +2752,10 @@
       <c r="A53" s="2">
         <v>39</v>
       </c>
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="C53" s="24"/>
+      <c r="C53" s="68"/>
       <c r="D53" s="9" t="s">
         <v>13</v>
       </c>
@@ -2764,10 +2764,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G53" s="25" t="s">
+      <c r="G53" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="H53" s="25"/>
+      <c r="H53" s="57"/>
       <c r="R53" s="12" t="s">
         <v>83</v>
       </c>
@@ -2776,10 +2776,10 @@
       <c r="A54" s="2">
         <v>40</v>
       </c>
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="65" t="s">
         <v>96</v>
       </c>
-      <c r="C54" s="24"/>
+      <c r="C54" s="68"/>
       <c r="D54" s="9" t="s">
         <v>6</v>
       </c>
@@ -2788,8 +2788,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
       <c r="R54" s="12" t="s">
         <v>83</v>
       </c>
@@ -2833,14 +2833,101 @@
       <c r="C63" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D63" s="17" t="s">
+      <c r="D63" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
+      <c r="E63" s="69"/>
+      <c r="F63" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="111">
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="C1:D3"/>
@@ -2865,93 +2952,6 @@
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <conditionalFormatting sqref="D58">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
@@ -3027,15 +3027,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100854852AB1FCCB343B38344B0B41716E7" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f3072bb31fb469f1da3162ac9bfbed5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1368c656-b5be-4b92-a170-f03a090da0eb" xmlns:ns3="09c4be65-2cf9-46da-869c-d5826f262cb1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b182ede65aa816d91ef00987d518e42" ns2:_="" ns3:_="">
     <xsd:import namespace="1368c656-b5be-4b92-a170-f03a090da0eb"/>
@@ -3278,6 +3269,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB296EE7-E205-4D20-97DE-474F1D44B89F}">
   <ds:schemaRefs>
@@ -3290,14 +3290,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C9098F7-9747-4B0C-A7F4-326F37B81062}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58522EE4-9543-446C-870D-236E82CB8943}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3314,4 +3306,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C9098F7-9747-4B0C-A7F4-326F37B81062}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>